<commit_message>
send image and text
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">Phone</t>
   </si>
@@ -41,6 +41,12 @@
   </si>
   <si>
     <t xml:space="preserve">Value2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roji</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Firman</t>
   </si>
 </sst>
 </file>
@@ -313,10 +319,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -357,6 +363,22 @@
         <v>6</v>
       </c>
     </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>6285695039087</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>6285717124020</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>